<commit_message>
240320 - finish reframe with Orchestrator
</commit_message>
<xml_diff>
--- a/UndatedPracticeDemo/Data/Config.xlsx
+++ b/UndatedPracticeDemo/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UipathWorkspace\Practice\UndatedPracticeDemo\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://lanxess1-my.sharepoint.com/personal/hank_peng_ext_lanxess_com/Documents/Desktop/HanqinpGit_UiPath/UiPath/UndatedPracticeDemo/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3938BE47-8405-4278-A755-F34AC844EA02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2880" yWindow="1728" windowWidth="17280" windowHeight="8976" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -564,7 +564,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>

</xml_diff>